<commit_message>
td and cour tell functions
</commit_message>
<xml_diff>
--- a/data/schdls/cpi2.xlsx
+++ b/data/schdls/cpi2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t xml:space="preserve">Sunday</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cours Analyse 3 Mr Bouabdallah Amphi.C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty</t>
   </si>
   <si>
     <t xml:space="preserve">TD G1 Algèbre3 S1 Mekri</t>
@@ -208,8 +211,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,39 +333,54 @@
       <c r="C6" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>25</v>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
speaker of modules Td / Cour by day and speaker of td by day and time of it
</commit_message>
<xml_diff>
--- a/data/schdls/cpi2.xlsx
+++ b/data/schdls/cpi2.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="g1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="g2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="g3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -211,8 +213,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -393,4 +395,56 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>